<commit_message>
Refactor delivery scheduling and reporting logic. Updated schedule CSV and Excel outputs to reflect new truck and store assignments, including improved cost calculations and service time adjustments. Enhanced logging for delivery notifications and schedule updates. Implemented temporary file handling for output to avoid conflicts with open files. Improved route planning to optimize for cost and delivery time.
</commit_message>
<xml_diff>
--- a/output/schedule.xlsx
+++ b/output/schedule.xlsx
@@ -62,145 +62,166 @@
     <t>ROUTE_1</t>
   </si>
   <si>
+    <t>TRUCK_003</t>
+  </si>
+  <si>
+    <t>08:00</t>
+  </si>
+  <si>
+    <t>18:00</t>
+  </si>
+  <si>
+    <t>STORE_002</t>
+  </si>
+  <si>
+    <t>PROD_004</t>
+  </si>
+  <si>
+    <t>09:30</t>
+  </si>
+  <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>PROD_005</t>
+  </si>
+  <si>
+    <t>PROD_006</t>
+  </si>
+  <si>
+    <t>ROUTE_2</t>
+  </si>
+  <si>
+    <t>TRUCK_007</t>
+  </si>
+  <si>
+    <t>STORE_004</t>
+  </si>
+  <si>
+    <t>PROD_008</t>
+  </si>
+  <si>
+    <t>09:00</t>
+  </si>
+  <si>
+    <t>09:15</t>
+  </si>
+  <si>
+    <t>PROD_009</t>
+  </si>
+  <si>
+    <t>ROUTE_3</t>
+  </si>
+  <si>
+    <t>TRUCK_001</t>
+  </si>
+  <si>
+    <t>STORE_005</t>
+  </si>
+  <si>
+    <t>PROD_002</t>
+  </si>
+  <si>
+    <t>11:00</t>
+  </si>
+  <si>
+    <t>11:18</t>
+  </si>
+  <si>
+    <t>PROD_010</t>
+  </si>
+  <si>
+    <t>ROUTE_4</t>
+  </si>
+  <si>
     <t>TRUCK_005</t>
   </si>
   <si>
-    <t>08:00</t>
-  </si>
-  <si>
-    <t>18:00</t>
-  </si>
-  <si>
-    <t>STORE_002</t>
-  </si>
-  <si>
-    <t>PROD_004</t>
-  </si>
-  <si>
-    <t>09:30</t>
-  </si>
-  <si>
-    <t>10:00</t>
-  </si>
-  <si>
-    <t>PROD_005</t>
-  </si>
-  <si>
-    <t>PROD_006</t>
-  </si>
-  <si>
-    <t>ROUTE_2</t>
+    <t>STORE_010</t>
+  </si>
+  <si>
+    <t>PROD_003</t>
+  </si>
+  <si>
+    <t>10:16</t>
+  </si>
+  <si>
+    <t>PROD_007</t>
+  </si>
+  <si>
+    <t>ROUTE_5</t>
+  </si>
+  <si>
+    <t>TRUCK_002</t>
+  </si>
+  <si>
+    <t>STORE_011</t>
+  </si>
+  <si>
+    <t>09:24</t>
+  </si>
+  <si>
+    <t>ROUTE_6</t>
   </si>
   <si>
     <t>TRUCK_006</t>
   </si>
   <si>
+    <t>STORE_012</t>
+  </si>
+  <si>
+    <t>11:19</t>
+  </si>
+  <si>
+    <t>ROUTE_7</t>
+  </si>
+  <si>
+    <t>TRUCK_004</t>
+  </si>
+  <si>
+    <t>STORE_001</t>
+  </si>
+  <si>
+    <t>PROD_001</t>
+  </si>
+  <si>
+    <t>09:23</t>
+  </si>
+  <si>
+    <t>ROUTE_8</t>
+  </si>
+  <si>
     <t>STORE_003</t>
   </si>
   <si>
-    <t>PROD_001</t>
-  </si>
-  <si>
-    <t>10:18</t>
-  </si>
-  <si>
-    <t>PROD_007</t>
-  </si>
-  <si>
-    <t>ROUTE_3</t>
-  </si>
-  <si>
-    <t>TRUCK_003</t>
-  </si>
-  <si>
-    <t>STORE_004</t>
-  </si>
-  <si>
-    <t>PROD_008</t>
-  </si>
-  <si>
-    <t>09:00</t>
-  </si>
-  <si>
-    <t>09:15</t>
-  </si>
-  <si>
-    <t>PROD_009</t>
-  </si>
-  <si>
-    <t>ROUTE_4</t>
-  </si>
-  <si>
-    <t>TRUCK_001</t>
-  </si>
-  <si>
-    <t>STORE_005</t>
-  </si>
-  <si>
-    <t>PROD_002</t>
-  </si>
-  <si>
-    <t>11:00</t>
-  </si>
-  <si>
-    <t>11:18</t>
-  </si>
-  <si>
-    <t>PROD_010</t>
-  </si>
-  <si>
-    <t>ROUTE_5</t>
-  </si>
-  <si>
-    <t>TRUCK_008</t>
-  </si>
-  <si>
-    <t>STORE_010</t>
-  </si>
-  <si>
-    <t>PROD_003</t>
-  </si>
-  <si>
-    <t>10:16</t>
-  </si>
-  <si>
-    <t>ROUTE_6</t>
-  </si>
-  <si>
-    <t>TRUCK_004</t>
-  </si>
-  <si>
-    <t>STORE_011</t>
-  </si>
-  <si>
-    <t>09:24</t>
-  </si>
-  <si>
-    <t>ROUTE_7</t>
-  </si>
-  <si>
-    <t>STORE_012</t>
-  </si>
-  <si>
-    <t>11:19</t>
-  </si>
-  <si>
-    <t>ROUTE_8</t>
-  </si>
-  <si>
-    <t>STORE_001</t>
+    <t>10:01</t>
   </si>
   <si>
     <t>10:19</t>
   </si>
   <si>
-    <t>10:42</t>
-  </si>
-  <si>
     <t>ROUTE_9</t>
   </si>
   <si>
-    <t>TRUCK_007</t>
+    <t>STORE_007</t>
+  </si>
+  <si>
+    <t>09:16</t>
+  </si>
+  <si>
+    <t>09:37</t>
+  </si>
+  <si>
+    <t>ROUTE_10</t>
+  </si>
+  <si>
+    <t>STORE_008</t>
+  </si>
+  <si>
+    <t>11:52</t>
+  </si>
+  <si>
+    <t>ROUTE_11</t>
   </si>
   <si>
     <t>STORE_006</t>
@@ -212,37 +233,16 @@
     <t>10:49</t>
   </si>
   <si>
-    <t>ROUTE_10</t>
-  </si>
-  <si>
-    <t>STORE_007</t>
-  </si>
-  <si>
-    <t>09:16</t>
-  </si>
-  <si>
-    <t>09:37</t>
-  </si>
-  <si>
-    <t>ROUTE_11</t>
-  </si>
-  <si>
-    <t>STORE_008</t>
-  </si>
-  <si>
-    <t>11:52</t>
-  </si>
-  <si>
     <t>ROUTE_12</t>
   </si>
   <si>
     <t>STORE_009</t>
   </si>
   <si>
-    <t>11:20</t>
-  </si>
-  <si>
-    <t>11:45</t>
+    <t>09:38</t>
+  </si>
+  <si>
+    <t>10:03</t>
   </si>
   <si>
     <t>ИТОГИ</t>
@@ -459,7 +459,7 @@
         <v>86.02162633521314</v>
       </c>
       <c r="O2" t="n" s="4">
-        <v>946.2378896873446</v>
+        <v>843.0119380850889</v>
       </c>
     </row>
     <row r="3">
@@ -506,7 +506,7 @@
         <v>86.02162633521314</v>
       </c>
       <c r="O3" t="n" s="4">
-        <v>946.2378896873446</v>
+        <v>843.0119380850889</v>
       </c>
     </row>
     <row r="4">
@@ -553,7 +553,7 @@
         <v>86.02162633521314</v>
       </c>
       <c r="O4" t="n" s="4">
-        <v>946.2378896873446</v>
+        <v>843.0119380850889</v>
       </c>
     </row>
     <row r="5">
@@ -573,34 +573,34 @@
         <v>27</v>
       </c>
       <c r="F5" t="n" s="3">
-        <v>15.0</v>
+        <v>30.0</v>
       </c>
       <c r="G5" t="n" s="3">
-        <v>40.0</v>
+        <v>10.0</v>
       </c>
       <c r="H5" t="s">
         <v>28</v>
       </c>
       <c r="I5" t="n" s="5">
-        <v>12.0</v>
+        <v>4.0</v>
       </c>
       <c r="J5" t="n" s="3">
         <v>6.0</v>
       </c>
       <c r="K5" t="n" s="3">
-        <v>42.72</v>
+        <v>31.62</v>
       </c>
       <c r="L5" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="M5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N5" t="n" s="3">
-        <v>85.44001872658765</v>
+        <v>63.242776601683794</v>
       </c>
       <c r="O5" t="n" s="4">
-        <v>1110.7202434456394</v>
+        <v>632.427766016838</v>
       </c>
     </row>
     <row r="6">
@@ -620,42 +620,42 @@
         <v>27</v>
       </c>
       <c r="F6" t="n" s="3">
-        <v>15.0</v>
+        <v>30.0</v>
       </c>
       <c r="G6" t="n" s="3">
-        <v>40.0</v>
+        <v>10.0</v>
       </c>
       <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="n" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="J6" t="n" s="3">
+        <v>4.800000000000001</v>
+      </c>
+      <c r="K6" t="n" s="3">
+        <v>31.62</v>
+      </c>
+      <c r="L6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" t="s">
         <v>30</v>
       </c>
-      <c r="I6" t="n" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="J6" t="n" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="K6" t="n" s="3">
-        <v>42.72</v>
-      </c>
-      <c r="L6" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" t="s">
-        <v>29</v>
-      </c>
       <c r="N6" t="n" s="3">
-        <v>85.44001872658765</v>
+        <v>63.242776601683794</v>
       </c>
       <c r="O6" t="n" s="4">
-        <v>1110.7202434456394</v>
+        <v>632.427766016838</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
@@ -664,45 +664,45 @@
         <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F7" t="n" s="3">
-        <v>30.0</v>
+        <v>5.0</v>
       </c>
       <c r="G7" t="n" s="3">
-        <v>10.0</v>
+        <v>45.0</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I7" t="n" s="5">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
       <c r="J7" t="n" s="3">
-        <v>6.0</v>
+        <v>2.4</v>
       </c>
       <c r="K7" t="n" s="3">
-        <v>31.62</v>
+        <v>45.28</v>
       </c>
       <c r="L7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N7" t="n" s="3">
-        <v>63.242776601683794</v>
+        <v>90.55692569068708</v>
       </c>
       <c r="O7" t="n" s="4">
-        <v>619.7792106965012</v>
+        <v>950.8477197522143</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
@@ -711,45 +711,45 @@
         <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F8" t="n" s="3">
-        <v>30.0</v>
+        <v>5.0</v>
       </c>
       <c r="G8" t="n" s="3">
-        <v>10.0</v>
+        <v>45.0</v>
       </c>
       <c r="H8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" t="n" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="J8" t="n" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="K8" t="n" s="3">
+        <v>45.28</v>
+      </c>
+      <c r="L8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8" t="s">
         <v>37</v>
       </c>
-      <c r="I8" t="n" s="5">
-        <v>6.0</v>
-      </c>
-      <c r="J8" t="n" s="3">
-        <v>4.800000000000001</v>
-      </c>
-      <c r="K8" t="n" s="3">
-        <v>31.62</v>
-      </c>
-      <c r="L8" t="s">
-        <v>35</v>
-      </c>
-      <c r="M8" t="s">
-        <v>36</v>
-      </c>
       <c r="N8" t="n" s="3">
-        <v>63.242776601683794</v>
+        <v>90.55692569068708</v>
       </c>
       <c r="O8" t="n" s="4">
-        <v>619.7792106965012</v>
+        <v>950.8477197522143</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
@@ -758,45 +758,45 @@
         <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F9" t="n" s="3">
-        <v>5.0</v>
+        <v>28.0</v>
       </c>
       <c r="G9" t="n" s="3">
-        <v>45.0</v>
+        <v>22.0</v>
       </c>
       <c r="H9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I9" t="n" s="5">
         <v>8.0</v>
       </c>
       <c r="J9" t="n" s="3">
-        <v>2.4</v>
+        <v>3.2</v>
       </c>
       <c r="K9" t="n" s="3">
-        <v>45.28</v>
+        <v>35.61</v>
       </c>
       <c r="L9" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="M9" t="s">
         <v>43</v>
       </c>
       <c r="N9" t="n" s="3">
-        <v>90.55692569068708</v>
+        <v>71.21898762952972</v>
       </c>
       <c r="O9" t="n" s="4">
-        <v>950.8477197522143</v>
+        <v>783.408863924827</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
@@ -805,37 +805,37 @@
         <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F10" t="n" s="3">
-        <v>5.0</v>
+        <v>28.0</v>
       </c>
       <c r="G10" t="n" s="3">
-        <v>45.0</v>
+        <v>22.0</v>
       </c>
       <c r="H10" t="s">
         <v>44</v>
       </c>
       <c r="I10" t="n" s="5">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="J10" t="n" s="3">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="K10" t="n" s="3">
-        <v>45.28</v>
+        <v>35.61</v>
       </c>
       <c r="L10" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="M10" t="s">
         <v>43</v>
       </c>
       <c r="N10" t="n" s="3">
-        <v>90.55692569068708</v>
+        <v>71.21898762952972</v>
       </c>
       <c r="O10" t="n" s="4">
-        <v>950.8477197522143</v>
+        <v>783.408863924827</v>
       </c>
     </row>
     <row r="11">
@@ -855,34 +855,34 @@
         <v>47</v>
       </c>
       <c r="F11" t="n" s="3">
-        <v>28.0</v>
+        <v>18.0</v>
       </c>
       <c r="G11" t="n" s="3">
-        <v>22.0</v>
+        <v>38.0</v>
       </c>
       <c r="H11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" t="n" s="5">
+        <v>12.0</v>
+      </c>
+      <c r="J11" t="n" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="K11" t="n" s="3">
+        <v>42.05</v>
+      </c>
+      <c r="L11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" t="s">
         <v>48</v>
       </c>
-      <c r="I11" t="n" s="5">
-        <v>8.0</v>
-      </c>
-      <c r="J11" t="n" s="3">
-        <v>3.2</v>
-      </c>
-      <c r="K11" t="n" s="3">
-        <v>35.61</v>
-      </c>
-      <c r="L11" t="s">
-        <v>22</v>
-      </c>
-      <c r="M11" t="s">
-        <v>49</v>
-      </c>
       <c r="N11" t="n" s="3">
-        <v>71.21898762952972</v>
+        <v>84.09759208325727</v>
       </c>
       <c r="O11" t="n" s="4">
-        <v>1068.2848144429458</v>
+        <v>1009.1711049990872</v>
       </c>
     </row>
     <row r="12">
@@ -902,136 +902,136 @@
         <v>47</v>
       </c>
       <c r="F12" t="n" s="3">
-        <v>28.0</v>
+        <v>18.0</v>
       </c>
       <c r="G12" t="n" s="3">
-        <v>22.0</v>
+        <v>38.0</v>
       </c>
       <c r="H12" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="I12" t="n" s="5">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="J12" t="n" s="3">
-        <v>6.0</v>
+        <v>4.2</v>
       </c>
       <c r="K12" t="n" s="3">
-        <v>35.61</v>
+        <v>42.05</v>
       </c>
       <c r="L12" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="M12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N12" t="n" s="3">
-        <v>71.21898762952972</v>
+        <v>84.09759208325727</v>
       </c>
       <c r="O12" t="n" s="4">
-        <v>1068.2848144429458</v>
+        <v>1009.1711049990872</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
         <v>50</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
         <v>51</v>
       </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F13" t="n" s="3">
+        <v>42.0</v>
+      </c>
+      <c r="G13" t="n" s="3">
+        <v>18.0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" t="n" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="J13" t="n" s="3">
+        <v>2.6999999999999997</v>
+      </c>
+      <c r="K13" t="n" s="3">
+        <v>45.69</v>
+      </c>
+      <c r="L13" t="s">
+        <v>36</v>
+      </c>
+      <c r="M13" t="s">
         <v>52</v>
       </c>
-      <c r="F13" t="n" s="3">
-        <v>18.0</v>
-      </c>
-      <c r="G13" t="n" s="3">
-        <v>38.0</v>
-      </c>
-      <c r="H13" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" t="n" s="5">
-        <v>12.0</v>
-      </c>
-      <c r="J13" t="n" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="K13" t="n" s="3">
-        <v>42.05</v>
-      </c>
-      <c r="L13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M13" t="s">
-        <v>53</v>
-      </c>
       <c r="N13" t="n" s="3">
-        <v>84.09759208325727</v>
+        <v>91.38463863518345</v>
       </c>
       <c r="O13" t="n" s="4">
-        <v>1219.4150852072303</v>
+        <v>1188.0003022573849</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
         <v>50</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
         <v>51</v>
       </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="F14" t="n" s="3">
+        <v>42.0</v>
+      </c>
+      <c r="G14" t="n" s="3">
+        <v>18.0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" t="n" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="J14" t="n" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="K14" t="n" s="3">
+        <v>45.69</v>
+      </c>
+      <c r="L14" t="s">
+        <v>36</v>
+      </c>
+      <c r="M14" t="s">
         <v>52</v>
       </c>
-      <c r="F14" t="n" s="3">
-        <v>18.0</v>
-      </c>
-      <c r="G14" t="n" s="3">
-        <v>38.0</v>
-      </c>
-      <c r="H14" t="s">
-        <v>44</v>
-      </c>
-      <c r="I14" t="n" s="5">
-        <v>7.0</v>
-      </c>
-      <c r="J14" t="n" s="3">
-        <v>4.2</v>
-      </c>
-      <c r="K14" t="n" s="3">
-        <v>42.05</v>
-      </c>
-      <c r="L14" t="s">
-        <v>35</v>
-      </c>
-      <c r="M14" t="s">
-        <v>53</v>
-      </c>
       <c r="N14" t="n" s="3">
-        <v>84.09759208325727</v>
+        <v>91.38463863518345</v>
       </c>
       <c r="O14" t="n" s="4">
-        <v>1219.4150852072303</v>
+        <v>1188.0003022573849</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
         <v>54</v>
-      </c>
-      <c r="B15" t="s">
-        <v>16</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
@@ -1043,42 +1043,42 @@
         <v>55</v>
       </c>
       <c r="F15" t="n" s="3">
-        <v>42.0</v>
+        <v>10.0</v>
       </c>
       <c r="G15" t="n" s="3">
-        <v>18.0</v>
+        <v>20.0</v>
       </c>
       <c r="H15" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="I15" t="n" s="5">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="J15" t="n" s="3">
-        <v>2.6999999999999997</v>
+        <v>5.0</v>
       </c>
       <c r="K15" t="n" s="3">
-        <v>45.69</v>
+        <v>22.36</v>
       </c>
       <c r="L15" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="M15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N15" t="n" s="3">
-        <v>91.38463863518345</v>
+        <v>44.7206797749979</v>
       </c>
       <c r="O15" t="n" s="4">
-        <v>1005.2310249870179</v>
+        <v>648.4498567374695</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
         <v>54</v>
-      </c>
-      <c r="B16" t="s">
-        <v>16</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
@@ -1090,42 +1090,42 @@
         <v>55</v>
       </c>
       <c r="F16" t="n" s="3">
-        <v>42.0</v>
+        <v>10.0</v>
       </c>
       <c r="G16" t="n" s="3">
-        <v>18.0</v>
+        <v>20.0</v>
       </c>
       <c r="H16" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="I16" t="n" s="5">
         <v>5.0</v>
       </c>
       <c r="J16" t="n" s="3">
-        <v>5.0</v>
+        <v>1.5</v>
       </c>
       <c r="K16" t="n" s="3">
-        <v>45.69</v>
+        <v>22.36</v>
       </c>
       <c r="L16" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="M16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N16" t="n" s="3">
-        <v>91.38463863518345</v>
+        <v>44.7206797749979</v>
       </c>
       <c r="O16" t="n" s="4">
-        <v>1005.2310249870179</v>
+        <v>648.4498567374695</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -1134,7 +1134,7 @@
         <v>18</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F17" t="n" s="3">
         <v>10.0</v>
@@ -1143,36 +1143,36 @@
         <v>20.0</v>
       </c>
       <c r="H17" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="I17" t="n" s="5">
-        <v>10.0</v>
+        <v>3.0</v>
       </c>
       <c r="J17" t="n" s="3">
-        <v>5.0</v>
+        <v>1.2000000000000002</v>
       </c>
       <c r="K17" t="n" s="3">
         <v>22.36</v>
       </c>
       <c r="L17" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="M17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N17" t="n" s="3">
         <v>44.7206797749979</v>
       </c>
       <c r="O17" t="n" s="4">
-        <v>581.3688370749727</v>
+        <v>648.4498567374695</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
@@ -1181,45 +1181,45 @@
         <v>18</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F18" t="n" s="3">
-        <v>10.0</v>
+        <v>15.0</v>
       </c>
       <c r="G18" t="n" s="3">
-        <v>20.0</v>
+        <v>40.0</v>
       </c>
       <c r="H18" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="I18" t="n" s="5">
-        <v>5.0</v>
+        <v>12.0</v>
       </c>
       <c r="J18" t="n" s="3">
-        <v>1.5</v>
+        <v>6.0</v>
       </c>
       <c r="K18" t="n" s="3">
-        <v>22.36</v>
+        <v>42.72</v>
       </c>
       <c r="L18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="M18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="N18" t="n" s="3">
-        <v>44.7206797749979</v>
+        <v>85.44001872658765</v>
       </c>
       <c r="O18" t="n" s="4">
-        <v>581.3688370749727</v>
+        <v>837.3121835205591</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
@@ -1228,45 +1228,45 @@
         <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F19" t="n" s="3">
-        <v>10.0</v>
+        <v>15.0</v>
       </c>
       <c r="G19" t="n" s="3">
-        <v>20.0</v>
+        <v>40.0</v>
       </c>
       <c r="H19" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I19" t="n" s="5">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="J19" t="n" s="3">
-        <v>1.2000000000000002</v>
+        <v>2.0</v>
       </c>
       <c r="K19" t="n" s="3">
-        <v>22.36</v>
+        <v>42.72</v>
       </c>
       <c r="L19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="M19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="N19" t="n" s="3">
-        <v>44.7206797749979</v>
+        <v>85.44001872658765</v>
       </c>
       <c r="O19" t="n" s="4">
-        <v>581.3688370749727</v>
+        <v>837.3121835205591</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
@@ -1278,22 +1278,22 @@
         <v>63</v>
       </c>
       <c r="F20" t="n" s="3">
-        <v>40.0</v>
+        <v>20.0</v>
       </c>
       <c r="G20" t="n" s="3">
-        <v>25.0</v>
+        <v>30.0</v>
       </c>
       <c r="H20" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I20" t="n" s="5">
-        <v>7.0</v>
+        <v>10.0</v>
       </c>
       <c r="J20" t="n" s="3">
-        <v>3.5</v>
+        <v>3.0</v>
       </c>
       <c r="K20" t="n" s="3">
-        <v>47.17</v>
+        <v>36.06</v>
       </c>
       <c r="L20" t="s">
         <v>64</v>
@@ -1302,18 +1302,18 @@
         <v>65</v>
       </c>
       <c r="N20" t="n" s="3">
-        <v>94.33990566028302</v>
+        <v>72.1155127546399</v>
       </c>
       <c r="O20" t="n" s="4">
-        <v>943.3990566028302</v>
+        <v>721.155127546399</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
@@ -1325,22 +1325,22 @@
         <v>63</v>
       </c>
       <c r="F21" t="n" s="3">
-        <v>40.0</v>
+        <v>20.0</v>
       </c>
       <c r="G21" t="n" s="3">
-        <v>25.0</v>
+        <v>30.0</v>
       </c>
       <c r="H21" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="I21" t="n" s="5">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="J21" t="n" s="3">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="K21" t="n" s="3">
-        <v>47.17</v>
+        <v>36.06</v>
       </c>
       <c r="L21" t="s">
         <v>64</v>
@@ -1349,18 +1349,18 @@
         <v>65</v>
       </c>
       <c r="N21" t="n" s="3">
-        <v>94.33990566028302</v>
+        <v>72.1155127546399</v>
       </c>
       <c r="O21" t="n" s="4">
-        <v>943.3990566028302</v>
+        <v>721.155127546399</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
@@ -1369,37 +1369,37 @@
         <v>18</v>
       </c>
       <c r="E22" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F22" t="n" s="3">
-        <v>40.0</v>
+        <v>35.0</v>
       </c>
       <c r="G22" t="n" s="3">
-        <v>25.0</v>
+        <v>15.0</v>
       </c>
       <c r="H22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I22" t="n" s="5">
-        <v>3.0</v>
+        <v>20.0</v>
       </c>
       <c r="J22" t="n" s="3">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="K22" t="n" s="3">
-        <v>47.17</v>
+        <v>38.08</v>
       </c>
       <c r="L22" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="M22" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="N22" t="n" s="3">
-        <v>94.33990566028302</v>
+        <v>76.15886552931954</v>
       </c>
       <c r="O22" t="n" s="4">
-        <v>943.3990566028302</v>
+        <v>799.6680880578551</v>
       </c>
     </row>
     <row r="23">
@@ -1407,7 +1407,7 @@
         <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
@@ -1419,42 +1419,42 @@
         <v>67</v>
       </c>
       <c r="F23" t="n" s="3">
-        <v>20.0</v>
+        <v>35.0</v>
       </c>
       <c r="G23" t="n" s="3">
-        <v>30.0</v>
+        <v>15.0</v>
       </c>
       <c r="H23" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="I23" t="n" s="5">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="J23" t="n" s="3">
-        <v>3.0</v>
+        <v>12.0</v>
       </c>
       <c r="K23" t="n" s="3">
-        <v>36.06</v>
+        <v>38.08</v>
       </c>
       <c r="L23" t="s">
+        <v>52</v>
+      </c>
+      <c r="M23" t="s">
         <v>68</v>
       </c>
-      <c r="M23" t="s">
-        <v>69</v>
-      </c>
       <c r="N23" t="n" s="3">
-        <v>72.1155127546399</v>
+        <v>76.15886552931954</v>
       </c>
       <c r="O23" t="n" s="4">
-        <v>706.732024995471</v>
+        <v>799.6680880578551</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
@@ -1463,131 +1463,131 @@
         <v>18</v>
       </c>
       <c r="E24" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F24" t="n" s="3">
-        <v>20.0</v>
+        <v>40.0</v>
       </c>
       <c r="G24" t="n" s="3">
-        <v>30.0</v>
+        <v>25.0</v>
       </c>
       <c r="H24" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="I24" t="n" s="5">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="J24" t="n" s="3">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="K24" t="n" s="3">
-        <v>36.06</v>
+        <v>47.17</v>
       </c>
       <c r="L24" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="M24" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="N24" t="n" s="3">
-        <v>72.1155127546399</v>
+        <v>94.33990566028302</v>
       </c>
       <c r="O24" t="n" s="4">
-        <v>706.732024995471</v>
+        <v>924.5310754707737</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" t="s">
         <v>70</v>
       </c>
-      <c r="B25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="F25" t="n" s="3">
+        <v>40.0</v>
+      </c>
+      <c r="G25" t="n" s="3">
+        <v>25.0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>42</v>
+      </c>
+      <c r="I25" t="n" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="J25" t="n" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="K25" t="n" s="3">
+        <v>47.17</v>
+      </c>
+      <c r="L25" t="s">
         <v>71</v>
-      </c>
-      <c r="F25" t="n" s="3">
-        <v>35.0</v>
-      </c>
-      <c r="G25" t="n" s="3">
-        <v>15.0</v>
-      </c>
-      <c r="H25" t="s">
-        <v>23</v>
-      </c>
-      <c r="I25" t="n" s="5">
-        <v>20.0</v>
-      </c>
-      <c r="J25" t="n" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="K25" t="n" s="3">
-        <v>38.08</v>
-      </c>
-      <c r="L25" t="s">
-        <v>56</v>
       </c>
       <c r="M25" t="s">
         <v>72</v>
       </c>
       <c r="N25" t="n" s="3">
-        <v>76.15886552931954</v>
+        <v>94.33990566028302</v>
       </c>
       <c r="O25" t="n" s="4">
-        <v>799.6680880578551</v>
+        <v>924.5310754707737</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" t="s">
         <v>70</v>
       </c>
-      <c r="B26" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="F26" t="n" s="3">
+        <v>40.0</v>
+      </c>
+      <c r="G26" t="n" s="3">
+        <v>25.0</v>
+      </c>
+      <c r="H26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" t="n" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="J26" t="n" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="K26" t="n" s="3">
+        <v>47.17</v>
+      </c>
+      <c r="L26" t="s">
         <v>71</v>
-      </c>
-      <c r="F26" t="n" s="3">
-        <v>35.0</v>
-      </c>
-      <c r="G26" t="n" s="3">
-        <v>15.0</v>
-      </c>
-      <c r="H26" t="s">
-        <v>34</v>
-      </c>
-      <c r="I26" t="n" s="5">
-        <v>8.0</v>
-      </c>
-      <c r="J26" t="n" s="3">
-        <v>12.0</v>
-      </c>
-      <c r="K26" t="n" s="3">
-        <v>38.08</v>
-      </c>
-      <c r="L26" t="s">
-        <v>56</v>
       </c>
       <c r="M26" t="s">
         <v>72</v>
       </c>
       <c r="N26" t="n" s="3">
-        <v>76.15886552931954</v>
+        <v>94.33990566028302</v>
       </c>
       <c r="O26" t="n" s="4">
-        <v>799.6680880578551</v>
+        <v>924.5310754707737</v>
       </c>
     </row>
     <row r="27">
@@ -1595,7 +1595,7 @@
         <v>73</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C27" t="s">
         <v>17</v>
@@ -1613,7 +1613,7 @@
         <v>28.0</v>
       </c>
       <c r="H27" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="I27" t="n" s="5">
         <v>15.0</v>
@@ -1634,7 +1634,7 @@
         <v>60.923092423455635</v>
       </c>
       <c r="O27" t="n" s="4">
-        <v>670.154016658012</v>
+        <v>609.2309242345564</v>
       </c>
     </row>
     <row r="28">
@@ -1642,7 +1642,7 @@
         <v>73</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
         <v>17</v>
@@ -1660,7 +1660,7 @@
         <v>28.0</v>
       </c>
       <c r="H28" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="I28" t="n" s="5">
         <v>5.0</v>
@@ -1681,7 +1681,7 @@
         <v>60.923092423455635</v>
       </c>
       <c r="O28" t="n" s="4">
-        <v>670.154016658012</v>
+        <v>609.2309242345564</v>
       </c>
     </row>
     <row r="31">
@@ -1694,7 +1694,7 @@
         <v>78</v>
       </c>
       <c r="B32" t="n" s="3">
-        <v>920.220621844838</v>
+        <v>920.2206218448381</v>
       </c>
     </row>
     <row r="33">
@@ -1702,7 +1702,7 @@
         <v>79</v>
       </c>
       <c r="B33" t="n" s="4">
-        <v>10621.838011608035</v>
+        <v>9947.214950603053</v>
       </c>
     </row>
     <row r="34">

</xml_diff>